<commit_message>
Fixed the products bug, made this compatible with links.txt
</commit_message>
<xml_diff>
--- a/src/trackers.py/price_tracker.xlsx
+++ b/src/trackers.py/price_tracker.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -49,9 +48,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,17 +426,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>45535.07559569624</v>
+      <c r="A1" s="2" t="n">
+        <v>45535.82706789798</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Canon R100 Mirrorless Camera</t>
+          <t>AULA F87 Wireless Mechanical Keyboard,75% TKL Gasket Custom Hot Swappable Keyboard,2.4Ghz/Type-C/Bluetooth Gaming Keyboard,Pre-lubed Switch RGB Backlit Keyboard (Smoke Blue, Grey Wood Switch)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>₹90990.0</t>
+          <t>₹5999.0</t>
         </is>
       </c>
     </row>

</xml_diff>